<commit_message>
all test cases executed and updated the test_cases excel file
</commit_message>
<xml_diff>
--- a/4_Test_Cases/Test_Cases.xlsx
+++ b/4_Test_Cases/Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\service-marketplace-manual-qa\4_Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5331AC-499A-4C6F-A9E7-3014C3ECEC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7368F8-746E-4B2C-B4D8-0B11DB2E0223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="118">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -370,6 +370,15 @@
   </si>
   <si>
     <t>Notification received</t>
+  </si>
+  <si>
+    <t>User registered successfully and confirmation notification received</t>
+  </si>
+  <si>
+    <t>Error of validation is showing.</t>
+  </si>
+  <si>
+    <t>user logged in and notification for the login can be seen.</t>
   </si>
 </sst>
 </file>
@@ -737,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +760,7 @@
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,7 +824,9 @@
       <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
@@ -847,7 +859,9 @@
       <c r="H3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
@@ -880,7 +894,9 @@
       <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>